<commit_message>
USB Host HID 추가
</commit_message>
<xml_diff>
--- a/stm32f746_gfx/src/ap/TouchGFX/assets/texts/texts.xlsx
+++ b/stm32f746_gfx/src/ap/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4400" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10104" uniqueCount="160">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -339,6 +339,162 @@
   </si>
   <si>
     <t xml:space="preserve">115200  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB HID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_X : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_X : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_ : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_Y : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_X : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_X : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_Y : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_U : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_D : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_LtextArea_L_X.invalidate(); : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_L : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_R : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_L  : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_U : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_D : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_R : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_L : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disconnected </t>
   </si>
 </sst>
 </file>
@@ -1999,33 +2155,465 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:10"/>
-    <row r="14" spans="2:10"/>
-    <row r="15" spans="2:10"/>
-    <row r="16" spans="2:10"/>
-    <row r="17" spans="4:4"/>
-    <row r="18" spans="4:4"/>
-    <row r="19" spans="4:4"/>
-    <row r="20" spans="4:4"/>
-    <row r="21" spans="4:4"/>
-    <row r="22" spans="4:4"/>
-    <row r="23" spans="4:4"/>
-    <row r="24" spans="4:4"/>
-    <row r="25" spans="4:4"/>
-    <row r="26" spans="4:4"/>
-    <row r="27" spans="4:4"/>
-    <row r="28" spans="4:4"/>
-    <row r="29" spans="4:4"/>
-    <row r="30" spans="4:4"/>
-    <row r="31" spans="4:4"/>
-    <row r="32" spans="4:4"/>
-    <row r="33" spans="4:4"/>
-    <row r="34" spans="4:4"/>
-    <row r="35" spans="4:4"/>
-    <row r="36" spans="4:4"/>
-    <row r="37" spans="4:4"/>
-    <row r="38" spans="4:4"/>
-    <row r="39" spans="4:4"/>
+    <row r="13" spans="2:10">
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="B23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="B24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="B25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="B27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="B28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="B29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="B30" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="B31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="B32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="B33" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="B34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>154</v>
+      </c>
+      <c r="F34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="B35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="B36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>153</v>
+      </c>
+      <c r="F36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="B37" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="B38" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" t="s">
+        <v>158</v>
+      </c>
+      <c r="F38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="B39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" t="s">
+        <v>159</v>
+      </c>
+      <c r="F39" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="40" spans="4:4"/>
     <row r="41" spans="4:4"/>
     <row r="42" spans="4:4"/>

</xml_diff>